<commit_message>
edited tests w new processors
</commit_message>
<xml_diff>
--- a/use_case_content/compared_table.xlsx
+++ b/use_case_content/compared_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meltr\OneDrive\Documents\(APT2)\D4\STAGE\github\GenEval\libraries\content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meltr\OneDrive\Documents\(APT2)\D4\STAGE\github\GenEval\use_case_content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3B0DC7-2821-458E-A749-58A0EB6DB701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A66746D-137F-4D87-BE3B-1B3A7C3DEAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F9D2BD8B-06B9-4933-89D2-CDC21B310CAB}"/>
+    <workbookView xWindow="-3060" yWindow="-10980" windowWidth="13830" windowHeight="7590" xr2:uid="{F9D2BD8B-06B9-4933-89D2-CDC21B310CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t xml:space="preserve">Nb </t>
   </si>
@@ -129,6 +129,57 @@
   </si>
   <si>
     <t>DeFeEeGe</t>
+  </si>
+  <si>
+    <t>Bool</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>llm test</t>
+  </si>
+  <si>
+    <t>A or B</t>
+  </si>
+  <si>
+    <t>the meat is cooked</t>
+  </si>
+  <si>
+    <t>A and B</t>
+  </si>
+  <si>
+    <t>you should have it</t>
+  </si>
+  <si>
+    <t>i have 98 apples</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>D and C</t>
+  </si>
+  <si>
+    <t>hey</t>
+  </si>
+  <si>
+    <t>What's your name ?</t>
+  </si>
+  <si>
+    <t>I want Bacillus in the broccoli</t>
+  </si>
+  <si>
+    <t>the person comes from an European country and is young.</t>
+  </si>
+  <si>
+    <t>a fact about one's personality is described</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>microbiological tests were conducted in a supermarket.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +203,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -160,100 +211,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,137 +553,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FB56316-6D8E-4C13-8C97-192ED260E557}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>575</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>7</v>
-      </c>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>1000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
-        <v>575</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6">
+        <v>140</v>
+      </c>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="5"/>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>1000</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>34</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="8" t="s">
-        <v>21</v>
-      </c>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>